<commit_message>
Some final formatting changes
</commit_message>
<xml_diff>
--- a/Sanimal/Sanimal.xlsx
+++ b/Sanimal/Sanimal.xlsx
@@ -12,20 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Cardinal</t>
-  </si>
-  <si>
-    <t>Coyote</t>
-  </si>
-  <si>
-    <t>Bobcat</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -77,7 +64,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Species Accumulation</c:v>
+            <c:v>Data Table</c:v>
           </c:tx>
           <c:xVal>
             <c:numRef>
@@ -85,13 +72,13 @@
               <c:numCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -102,13 +89,13 @@
               <c:numCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -207,35 +194,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B1" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+        <v>3.0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+        <v>6.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="B3" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+        <v>9.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>